<commit_message>
UNION- extraccion de errores
</commit_message>
<xml_diff>
--- a/ItemsExtraer.xlsx
+++ b/ItemsExtraer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcolin\Documents\GitHub\Codigo-IMPEX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCEE72B-59E9-46F4-8C7D-F2DD345DBC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01973D0A-6DEC-4A9D-991E-B313F09CFD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A101"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -909,6 +909,16 @@
         <v>2206810102</v>
       </c>
     </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" s="4">
+        <v>2003674022</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3">
+        <v>200366800</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>